<commit_message>
Presentation and BOM update
</commit_message>
<xml_diff>
--- a/Hardware/FinalDesign/PrototypeBOM.xlsx
+++ b/Hardware/FinalDesign/PrototypeBOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Ver.2" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="242">
   <si>
     <t>Quantity</t>
   </si>
@@ -721,9 +721,6 @@
     <t>http://www.digikey.com/product-detail/en/ECS-160-20-33-TR/XC1137TR-ND/813224</t>
   </si>
   <si>
-    <t>http://www.digikey.com/classic/Ordering/AddPart.aspx?WT.z_cid=Shared_Cart</t>
-  </si>
-  <si>
     <t>LMV358IDGKR</t>
   </si>
   <si>
@@ -737,6 +734,18 @@
   </si>
   <si>
     <t>535-9541-1-ND</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>3/8 in pan head phillips</t>
+  </si>
+  <si>
+    <t>Sheet metal screws</t>
+  </si>
+  <si>
+    <t>16 pack</t>
   </si>
 </sst>
 </file>
@@ -746,7 +755,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -776,13 +785,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -895,7 +897,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="180">
+  <cellStyleXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1076,8 +1078,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1107,8 +1113,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1122,7 +1126,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="180">
+  <cellStyles count="184">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1216,6 +1220,8 @@
     <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1302,6 +1308,8 @@
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1631,10 +1639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S117"/>
+  <dimension ref="A1:S115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1682,7 +1690,7 @@
       <c r="A2" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="24" t="s">
         <v>180</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -1722,7 +1730,7 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="9"/>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C3" s="11"/>
@@ -1745,7 +1753,7 @@
         <v>0.12</v>
       </c>
       <c r="J3" s="12">
-        <f t="shared" ref="J3:J62" si="0">I3*H3</f>
+        <f t="shared" ref="J3:J60" si="0">I3*H3</f>
         <v>0.12</v>
       </c>
       <c r="K3" s="11" t="s">
@@ -1760,7 +1768,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="9"/>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C4" s="11"/>
@@ -1798,7 +1806,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="9"/>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="23" t="s">
         <v>183</v>
       </c>
       <c r="C5" s="11"/>
@@ -1836,7 +1844,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="14"/>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="25" t="s">
         <v>180</v>
       </c>
       <c r="C6" s="15"/>
@@ -1901,7 +1909,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="9"/>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C9" s="11" t="s">
@@ -1942,7 +1950,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="9"/>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C10" s="11"/>
@@ -1981,7 +1989,7 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" s="9"/>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C11" s="11"/>
@@ -2020,7 +2028,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="9"/>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C12" s="11"/>
@@ -2059,7 +2067,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="9"/>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C13" s="11"/>
@@ -2098,7 +2106,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="9"/>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C14" s="11"/>
@@ -2137,7 +2145,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="9"/>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C15" s="11"/>
@@ -2176,7 +2184,7 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="9"/>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C16" s="11"/>
@@ -2215,7 +2223,7 @@
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="9"/>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C17" s="11"/>
@@ -2254,7 +2262,7 @@
     </row>
     <row r="18" spans="1:19">
       <c r="A18" s="9"/>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C18" s="11"/>
@@ -2293,7 +2301,7 @@
     </row>
     <row r="19" spans="1:19">
       <c r="A19" s="9"/>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C19" s="11" t="s">
@@ -2334,7 +2342,7 @@
     </row>
     <row r="20" spans="1:19">
       <c r="A20" s="18"/>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="25" t="s">
         <v>183</v>
       </c>
       <c r="C20" s="15"/>
@@ -2400,7 +2408,7 @@
     </row>
     <row r="23" spans="1:19">
       <c r="A23" s="9"/>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C23" s="11"/>
@@ -2438,7 +2446,7 @@
     </row>
     <row r="24" spans="1:19">
       <c r="A24" s="14"/>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="25" t="s">
         <v>180</v>
       </c>
       <c r="C24" s="15"/>
@@ -2504,7 +2512,7 @@
     </row>
     <row r="27" spans="1:19">
       <c r="A27" s="9"/>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C27" s="11"/>
@@ -2515,10 +2523,10 @@
         <v>45</v>
       </c>
       <c r="F27" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="G27" t="s">
         <v>234</v>
-      </c>
-      <c r="G27" t="s">
-        <v>235</v>
       </c>
       <c r="H27" s="11">
         <v>1</v>
@@ -2531,7 +2539,7 @@
         <v>0.82</v>
       </c>
       <c r="K27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L27" s="11"/>
       <c r="M27" s="11"/>
@@ -2544,7 +2552,7 @@
     </row>
     <row r="28" spans="1:19">
       <c r="A28" s="9"/>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C28" s="11"/>
@@ -2584,7 +2592,7 @@
     </row>
     <row r="29" spans="1:19">
       <c r="A29" s="9"/>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C29" s="11"/>
@@ -2624,7 +2632,7 @@
     </row>
     <row r="30" spans="1:19">
       <c r="A30" s="9"/>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C30" s="11"/>
@@ -2664,7 +2672,7 @@
     </row>
     <row r="31" spans="1:19">
       <c r="A31" s="14"/>
-      <c r="B31" s="27" t="s">
+      <c r="B31" s="25" t="s">
         <v>180</v>
       </c>
       <c r="C31" s="15"/>
@@ -2730,7 +2738,7 @@
     </row>
     <row r="34" spans="1:18">
       <c r="A34" s="9"/>
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C34" s="11"/>
@@ -2768,7 +2776,7 @@
     </row>
     <row r="35" spans="1:18">
       <c r="A35" s="14"/>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="25" t="s">
         <v>180</v>
       </c>
       <c r="C35" s="15" t="s">
@@ -2836,7 +2844,7 @@
     </row>
     <row r="38" spans="1:18">
       <c r="A38" s="9"/>
-      <c r="B38" s="25" t="s">
+      <c r="B38" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C38" s="11"/>
@@ -2875,7 +2883,7 @@
     </row>
     <row r="39" spans="1:18">
       <c r="A39" s="9"/>
-      <c r="B39" s="25" t="s">
+      <c r="B39" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C39" s="11"/>
@@ -2953,7 +2961,7 @@
     </row>
     <row r="41" spans="1:18">
       <c r="A41" s="14"/>
-      <c r="B41" s="27" t="s">
+      <c r="B41" s="25" t="s">
         <v>180</v>
       </c>
       <c r="C41" s="15"/>
@@ -3019,7 +3027,7 @@
     </row>
     <row r="44" spans="1:18">
       <c r="A44" s="9"/>
-      <c r="B44" s="25" t="s">
+      <c r="B44" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C44" s="11"/>
@@ -3058,7 +3066,7 @@
     </row>
     <row r="45" spans="1:18">
       <c r="A45" s="14"/>
-      <c r="B45" s="27" t="s">
+      <c r="B45" s="25" t="s">
         <v>180</v>
       </c>
       <c r="C45" s="15"/>
@@ -3124,7 +3132,7 @@
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="1:18">
-      <c r="B48" s="28" t="s">
+      <c r="B48" s="26" t="s">
         <v>180</v>
       </c>
       <c r="D48" t="s">
@@ -3153,8 +3161,8 @@
         <v>160</v>
       </c>
     </row>
-    <row r="49" spans="2:11">
-      <c r="B49" s="28" t="s">
+    <row r="49" spans="1:11">
+      <c r="B49" s="26" t="s">
         <v>180</v>
       </c>
       <c r="D49" t="s">
@@ -3183,8 +3191,8 @@
         <v>232</v>
       </c>
     </row>
-    <row r="50" spans="2:11">
-      <c r="B50" s="28" t="s">
+    <row r="50" spans="1:11">
+      <c r="B50" s="26" t="s">
         <v>180</v>
       </c>
       <c r="D50" t="s">
@@ -3197,7 +3205,7 @@
         <v>23</v>
       </c>
       <c r="G50" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H50">
         <v>1</v>
@@ -3210,255 +3218,295 @@
         <v>2.34</v>
       </c>
       <c r="K50" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="51" spans="2:11">
-      <c r="B51" s="2"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-    </row>
-    <row r="52" spans="2:11">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" s="6" customFormat="1">
+      <c r="B51" s="5"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="20"/>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="3" t="s">
+        <v>238</v>
+      </c>
       <c r="B52" s="2"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="53" spans="2:11">
-      <c r="B53" s="2"/>
+    <row r="53" spans="1:11">
+      <c r="B53" s="26" t="s">
+        <v>180</v>
+      </c>
       <c r="D53" t="s">
-        <v>233</v>
-      </c>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-    </row>
-    <row r="54" spans="2:11" ht="20">
+        <v>229</v>
+      </c>
+      <c r="E53" t="s">
+        <v>156</v>
+      </c>
+      <c r="F53" t="s">
+        <v>22</v>
+      </c>
+      <c r="G53" t="s">
+        <v>157</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53" s="1">
+        <v>1.69</v>
+      </c>
+      <c r="J53" s="1">
+        <f t="shared" ref="J53" si="8">I53*H53</f>
+        <v>1.69</v>
+      </c>
+      <c r="K53" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="B54" s="2"/>
-      <c r="H54" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="I54" s="23"/>
-      <c r="J54" s="24">
-        <f>SUM(J2:J50)</f>
-        <v>45.69</v>
-      </c>
-    </row>
-    <row r="55" spans="2:11">
+      <c r="E54" t="s">
+        <v>239</v>
+      </c>
+      <c r="F54" t="s">
+        <v>240</v>
+      </c>
+      <c r="G54" t="s">
+        <v>241</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54" s="1">
+        <v>1</v>
+      </c>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="1:11">
       <c r="B55" s="2"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
     </row>
-    <row r="56" spans="2:11">
+    <row r="56" spans="1:11">
       <c r="B56" s="2"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-    </row>
-    <row r="57" spans="2:11">
+      <c r="C56" t="s">
+        <v>174</v>
+      </c>
+      <c r="E56" t="s">
+        <v>175</v>
+      </c>
+      <c r="F56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="J56" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="B57" s="2"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
-    </row>
-    <row r="58" spans="2:11">
+      <c r="C57" t="s">
+        <v>141</v>
+      </c>
+      <c r="E57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F57" t="s">
+        <v>14</v>
+      </c>
+      <c r="G57" t="s">
+        <v>117</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J57" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="K57" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="B58" s="2"/>
-      <c r="C58" t="s">
-        <v>174</v>
-      </c>
       <c r="E58" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="F58" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="G58" t="s">
+        <v>137</v>
       </c>
       <c r="H58">
         <v>1</v>
       </c>
+      <c r="I58" s="1">
+        <v>0.17</v>
+      </c>
       <c r="J58" s="1">
         <f t="shared" si="0"/>
+        <v>0.17</v>
+      </c>
+      <c r="K58" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="B59" s="2"/>
+      <c r="E59" t="s">
+        <v>58</v>
+      </c>
+      <c r="F59" t="s">
+        <v>17</v>
+      </c>
+      <c r="H59">
+        <v>2</v>
+      </c>
+      <c r="J59" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:11">
-      <c r="B59" s="2"/>
-      <c r="C59" t="s">
-        <v>141</v>
-      </c>
-      <c r="E59" t="s">
-        <v>109</v>
-      </c>
-      <c r="F59" t="s">
-        <v>14</v>
-      </c>
-      <c r="G59" t="s">
-        <v>117</v>
-      </c>
-      <c r="H59">
-        <v>1</v>
-      </c>
-      <c r="I59" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="J59" s="1">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="K59" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="60" spans="2:11">
+    <row r="60" spans="1:11">
       <c r="B60" s="2"/>
       <c r="E60" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="F60" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G60" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
       <c r="H60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I60" s="1">
-        <v>0.17</v>
+        <v>0.1</v>
       </c>
       <c r="J60" s="1">
         <f t="shared" si="0"/>
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
       <c r="K60" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="61" spans="2:11">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="B61" s="2"/>
-      <c r="E61" t="s">
-        <v>58</v>
-      </c>
-      <c r="F61" t="s">
-        <v>17</v>
-      </c>
-      <c r="H61">
-        <v>2</v>
-      </c>
       <c r="J61" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="2:11">
+        <f>SUM(J2:J60)</f>
+        <v>47.85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
       <c r="B62" s="2"/>
-      <c r="E62" t="s">
-        <v>61</v>
-      </c>
-      <c r="F62" t="s">
-        <v>4</v>
-      </c>
-      <c r="G62" t="s">
-        <v>63</v>
-      </c>
-      <c r="H62">
-        <v>2</v>
-      </c>
-      <c r="I62" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="J62" s="1">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="K62" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="63" spans="2:11">
-      <c r="B63" s="2"/>
-      <c r="J63" s="1">
-        <f>SUM(J2:J62)</f>
-        <v>91.85</v>
-      </c>
-    </row>
-    <row r="64" spans="2:11">
-      <c r="B64" s="2"/>
-    </row>
-    <row r="67" spans="7:9">
-      <c r="G67" t="s">
+    </row>
+    <row r="65" spans="7:9">
+      <c r="G65" t="s">
         <v>176</v>
       </c>
-      <c r="I67" s="1">
-        <f>SUM(I2:I62)</f>
-        <v>37.069999999999993</v>
+      <c r="I65" s="1">
+        <f>SUM(I2:I60)</f>
+        <v>39.759999999999991</v>
+      </c>
+    </row>
+    <row r="92" spans="9:11">
+      <c r="I92" t="s">
+        <v>70</v>
+      </c>
+      <c r="K92" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="93" spans="9:11">
+      <c r="I93" t="s">
+        <v>99</v>
+      </c>
+      <c r="K93" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="94" spans="9:11">
       <c r="I94" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="K94" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="95" spans="9:11">
       <c r="I95" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K95" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="96" spans="9:11">
       <c r="I96" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="K96" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="97" spans="9:11">
       <c r="I97" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="K97" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="98" spans="9:11">
       <c r="I98" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="K98" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="99" spans="9:11">
       <c r="I99" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K99" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="100" spans="9:11">
       <c r="I100" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="K100" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="101" spans="9:11">
       <c r="I101" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="K101" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="102" spans="9:11">
       <c r="I102" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="K102" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="103" spans="9:11">
@@ -3466,47 +3514,47 @@
         <v>101</v>
       </c>
       <c r="K103" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="104" spans="9:11">
       <c r="I104" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="K104" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="105" spans="9:11">
       <c r="I105" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="K105" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="106" spans="9:11">
       <c r="I106" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="K106" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="107" spans="9:11">
       <c r="I107" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="K107" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="108" spans="9:11">
-      <c r="I108" t="s">
-        <v>97</v>
+      <c r="I108">
+        <v>50</v>
       </c>
       <c r="K108" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="109" spans="9:11">
@@ -3514,7 +3562,7 @@
         <v>101</v>
       </c>
       <c r="K109" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="110" spans="9:11">
@@ -3522,15 +3570,15 @@
         <v>50</v>
       </c>
       <c r="K110" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="111" spans="9:11">
-      <c r="I111" t="s">
-        <v>101</v>
+      <c r="I111">
+        <v>120</v>
       </c>
       <c r="K111" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="112" spans="9:11">
@@ -3538,51 +3586,36 @@
         <v>50</v>
       </c>
       <c r="K112" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="113" spans="9:11">
       <c r="I113">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="K113" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="114" spans="9:11">
       <c r="I114">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="K114" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="115" spans="9:11">
-      <c r="I115">
-        <v>50</v>
+      <c r="I115" t="s">
+        <v>106</v>
       </c>
       <c r="K115" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="116" spans="9:11">
-      <c r="I116">
-        <v>120</v>
-      </c>
-      <c r="K116" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="117" spans="9:11">
-      <c r="I117" t="s">
-        <v>106</v>
-      </c>
-      <c r="K117" t="s">
         <v>96</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>